<commit_message>
Comienzo de frontend fin de sesión 27-1-2026
</commit_message>
<xml_diff>
--- a/inputs/Excel_Personal_2.1.xlsx
+++ b/inputs/Excel_Personal_2.1.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z30"/>
+  <dimension ref="A1:T30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -522,36 +522,6 @@
           <t>Actividad 4</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>EMPRESA 2</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>PUESTO 2</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>PERIODO 2</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>EMPRESA 3</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>PUESTO 3</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>PERIODO 3</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -586,62 +556,16 @@
         <v>980</v>
       </c>
       <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Backend Lead</t>
-        </is>
-      </c>
+      <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>Festina Group</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>julio 2023 - Actualidad (2 años 7 meses)</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>Backend Lead</t>
-        </is>
-      </c>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr"/>
       <c r="R2" t="inlineStr"/>
       <c r="S2" t="inlineStr"/>
       <c r="T2" t="inlineStr"/>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>Festina Group</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>Analista programador Java</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>septiembre 2019 - julio 2023 (3 años 11 meses)</t>
-        </is>
-      </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>Carver Advanced Systems S.L.</t>
-        </is>
-      </c>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t>Analista programador Java</t>
-        </is>
-      </c>
-      <c r="Z2" t="inlineStr">
-        <is>
-          <t>febrero 2018 - agosto 2019 (1 año 7 meses)</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -686,12 +610,6 @@
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr"/>
-      <c r="U3" t="inlineStr"/>
-      <c r="V3" t="inlineStr"/>
-      <c r="W3" t="inlineStr"/>
-      <c r="X3" t="inlineStr"/>
-      <c r="Y3" t="inlineStr"/>
-      <c r="Z3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -726,62 +644,16 @@
         <v>1215</v>
       </c>
       <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>Analista programador Java</t>
-        </is>
-      </c>
+      <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>Festina Group</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>febrero 2021 - Actualidad (5 años)</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>Analista programador Java</t>
-        </is>
-      </c>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr"/>
       <c r="R4" t="inlineStr"/>
       <c r="S4" t="inlineStr"/>
       <c r="T4" t="inlineStr"/>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>Festina Lotus S.A.</t>
-        </is>
-      </c>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>Analista Programador Java</t>
-        </is>
-      </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>junio 2007 - noviembre 2019 (12 años 6 meses)</t>
-        </is>
-      </c>
-      <c r="X4" t="inlineStr">
-        <is>
-          <t>Connecta Group</t>
-        </is>
-      </c>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t>Administrador Intranet</t>
-        </is>
-      </c>
-      <c r="Z4" t="inlineStr">
-        <is>
-          <t>octubre 2006 - junio 2007 (9 meses)</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -816,62 +688,16 @@
         <v>650</v>
       </c>
       <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>Senior Java Developer</t>
-        </is>
-      </c>
+      <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>Festina Group</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>Mayo 2023 - Actualidad (2 years 9 months)</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>Senior Java Developer</t>
-        </is>
-      </c>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr"/>
       <c r="R5" t="inlineStr"/>
       <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr"/>
-      <c r="U5" t="inlineStr">
-        <is>
-          <t>NTT DATA Europe &amp; Latam</t>
-        </is>
-      </c>
-      <c r="V5" t="inlineStr">
-        <is>
-          <t>Analista y Desarrollador Full Stack</t>
-        </is>
-      </c>
-      <c r="W5" t="inlineStr">
-        <is>
-          <t>Enero 2022 - Mayo 2023 (1 year 5 months)</t>
-        </is>
-      </c>
-      <c r="X5" t="inlineStr">
-        <is>
-          <t>- Rol referente técnico en varias de las aplicaciones desarrolladas.</t>
-        </is>
-      </c>
-      <c r="Y5" t="inlineStr">
-        <is>
-          <t>Desarrollador Full Stack</t>
-        </is>
-      </c>
-      <c r="Z5" t="inlineStr">
-        <is>
-          <t>Septiembre 2017 - Febrero 2022 (4 years 6 months)</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -906,62 +732,16 @@
         <v>750</v>
       </c>
       <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>Analista Programador</t>
-        </is>
-      </c>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>Festina Group</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>Septiembre 2019 - Actualidad (6 years 5 months)</t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>Analista Programador</t>
-        </is>
-      </c>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr"/>
       <c r="R6" t="inlineStr"/>
       <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr"/>
-      <c r="U6" t="inlineStr">
-        <is>
-          <t>Festina Group</t>
-        </is>
-      </c>
-      <c r="V6" t="inlineStr">
-        <is>
-          <t>Analista Programador en Fira BCN</t>
-        </is>
-      </c>
-      <c r="W6" t="inlineStr">
-        <is>
-          <t>Abril 2019 - Agosto 2019 (5 months)</t>
-        </is>
-      </c>
-      <c r="X6" t="inlineStr">
-        <is>
-          <t>T-Systems Iberia</t>
-        </is>
-      </c>
-      <c r="Y6" t="inlineStr">
-        <is>
-          <t>Analista Programador</t>
-        </is>
-      </c>
-      <c r="Z6" t="inlineStr">
-        <is>
-          <t>Octubre 2015 - Marzo 2019 (3 years 6 months)</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -996,62 +776,16 @@
         <v>570</v>
       </c>
       <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>Analsita programador</t>
-        </is>
-      </c>
+      <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>Festina Group</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>Marzo 2016 - Actualidad (9 years 11 months)</t>
-        </is>
-      </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>Analsita programador</t>
-        </is>
-      </c>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr"/>
       <c r="R7" t="inlineStr"/>
       <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr"/>
-      <c r="U7" t="inlineStr">
-        <is>
-          <t>K-LAGAN</t>
-        </is>
-      </c>
-      <c r="V7" t="inlineStr">
-        <is>
-          <t>Delphi/Java Developer</t>
-        </is>
-      </c>
-      <c r="W7" t="inlineStr">
-        <is>
-          <t>Octubre 2013 - Septiembre 2015 (2 years)</t>
-        </is>
-      </c>
-      <c r="X7" t="inlineStr">
-        <is>
-          <t>ANF AC</t>
-        </is>
-      </c>
-      <c r="Y7" t="inlineStr">
-        <is>
-          <t>analista programador</t>
-        </is>
-      </c>
-      <c r="Z7" t="inlineStr">
-        <is>
-          <t>Octubre 2012 - Octubre 2013 (1 year 1 month)</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1096,12 +830,6 @@
       <c r="R8" t="inlineStr"/>
       <c r="S8" t="inlineStr"/>
       <c r="T8" t="inlineStr"/>
-      <c r="U8" t="inlineStr"/>
-      <c r="V8" t="inlineStr"/>
-      <c r="W8" t="inlineStr"/>
-      <c r="X8" t="inlineStr"/>
-      <c r="Y8" t="inlineStr"/>
-      <c r="Z8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1146,12 +874,6 @@
       <c r="R9" t="inlineStr"/>
       <c r="S9" t="inlineStr"/>
       <c r="T9" t="inlineStr"/>
-      <c r="U9" t="inlineStr"/>
-      <c r="V9" t="inlineStr"/>
-      <c r="W9" t="inlineStr"/>
-      <c r="X9" t="inlineStr"/>
-      <c r="Y9" t="inlineStr"/>
-      <c r="Z9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1196,12 +918,6 @@
       <c r="R10" t="inlineStr"/>
       <c r="S10" t="inlineStr"/>
       <c r="T10" t="inlineStr"/>
-      <c r="U10" t="inlineStr"/>
-      <c r="V10" t="inlineStr"/>
-      <c r="W10" t="inlineStr"/>
-      <c r="X10" t="inlineStr"/>
-      <c r="Y10" t="inlineStr"/>
-      <c r="Z10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1246,12 +962,6 @@
       <c r="R11" t="inlineStr"/>
       <c r="S11" t="inlineStr"/>
       <c r="T11" t="inlineStr"/>
-      <c r="U11" t="inlineStr"/>
-      <c r="V11" t="inlineStr"/>
-      <c r="W11" t="inlineStr"/>
-      <c r="X11" t="inlineStr"/>
-      <c r="Y11" t="inlineStr"/>
-      <c r="Z11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1296,12 +1006,6 @@
       <c r="R12" t="inlineStr"/>
       <c r="S12" t="inlineStr"/>
       <c r="T12" t="inlineStr"/>
-      <c r="U12" t="inlineStr"/>
-      <c r="V12" t="inlineStr"/>
-      <c r="W12" t="inlineStr"/>
-      <c r="X12" t="inlineStr"/>
-      <c r="Y12" t="inlineStr"/>
-      <c r="Z12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1346,12 +1050,6 @@
       <c r="R13" t="inlineStr"/>
       <c r="S13" t="inlineStr"/>
       <c r="T13" t="inlineStr"/>
-      <c r="U13" t="inlineStr"/>
-      <c r="V13" t="inlineStr"/>
-      <c r="W13" t="inlineStr"/>
-      <c r="X13" t="inlineStr"/>
-      <c r="Y13" t="inlineStr"/>
-      <c r="Z13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1396,12 +1094,6 @@
       <c r="R14" t="inlineStr"/>
       <c r="S14" t="inlineStr"/>
       <c r="T14" t="inlineStr"/>
-      <c r="U14" t="inlineStr"/>
-      <c r="V14" t="inlineStr"/>
-      <c r="W14" t="inlineStr"/>
-      <c r="X14" t="inlineStr"/>
-      <c r="Y14" t="inlineStr"/>
-      <c r="Z14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1446,12 +1138,6 @@
       <c r="R15" t="inlineStr"/>
       <c r="S15" t="inlineStr"/>
       <c r="T15" t="inlineStr"/>
-      <c r="U15" t="inlineStr"/>
-      <c r="V15" t="inlineStr"/>
-      <c r="W15" t="inlineStr"/>
-      <c r="X15" t="inlineStr"/>
-      <c r="Y15" t="inlineStr"/>
-      <c r="Z15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1496,12 +1182,6 @@
       <c r="R16" t="inlineStr"/>
       <c r="S16" t="inlineStr"/>
       <c r="T16" t="inlineStr"/>
-      <c r="U16" t="inlineStr"/>
-      <c r="V16" t="inlineStr"/>
-      <c r="W16" t="inlineStr"/>
-      <c r="X16" t="inlineStr"/>
-      <c r="Y16" t="inlineStr"/>
-      <c r="Z16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1546,12 +1226,6 @@
       <c r="R17" t="inlineStr"/>
       <c r="S17" t="inlineStr"/>
       <c r="T17" t="inlineStr"/>
-      <c r="U17" t="inlineStr"/>
-      <c r="V17" t="inlineStr"/>
-      <c r="W17" t="inlineStr"/>
-      <c r="X17" t="inlineStr"/>
-      <c r="Y17" t="inlineStr"/>
-      <c r="Z17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1596,12 +1270,6 @@
       <c r="R18" t="inlineStr"/>
       <c r="S18" t="inlineStr"/>
       <c r="T18" t="inlineStr"/>
-      <c r="U18" t="inlineStr"/>
-      <c r="V18" t="inlineStr"/>
-      <c r="W18" t="inlineStr"/>
-      <c r="X18" t="inlineStr"/>
-      <c r="Y18" t="inlineStr"/>
-      <c r="Z18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1646,12 +1314,6 @@
       <c r="R19" t="inlineStr"/>
       <c r="S19" t="inlineStr"/>
       <c r="T19" t="inlineStr"/>
-      <c r="U19" t="inlineStr"/>
-      <c r="V19" t="inlineStr"/>
-      <c r="W19" t="inlineStr"/>
-      <c r="X19" t="inlineStr"/>
-      <c r="Y19" t="inlineStr"/>
-      <c r="Z19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1696,12 +1358,6 @@
       <c r="R20" t="inlineStr"/>
       <c r="S20" t="inlineStr"/>
       <c r="T20" t="inlineStr"/>
-      <c r="U20" t="inlineStr"/>
-      <c r="V20" t="inlineStr"/>
-      <c r="W20" t="inlineStr"/>
-      <c r="X20" t="inlineStr"/>
-      <c r="Y20" t="inlineStr"/>
-      <c r="Z20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1746,12 +1402,6 @@
       <c r="R21" t="inlineStr"/>
       <c r="S21" t="inlineStr"/>
       <c r="T21" t="inlineStr"/>
-      <c r="U21" t="inlineStr"/>
-      <c r="V21" t="inlineStr"/>
-      <c r="W21" t="inlineStr"/>
-      <c r="X21" t="inlineStr"/>
-      <c r="Y21" t="inlineStr"/>
-      <c r="Z21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1796,12 +1446,6 @@
       <c r="R22" t="inlineStr"/>
       <c r="S22" t="inlineStr"/>
       <c r="T22" t="inlineStr"/>
-      <c r="U22" t="inlineStr"/>
-      <c r="V22" t="inlineStr"/>
-      <c r="W22" t="inlineStr"/>
-      <c r="X22" t="inlineStr"/>
-      <c r="Y22" t="inlineStr"/>
-      <c r="Z22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1846,12 +1490,6 @@
       <c r="R23" t="inlineStr"/>
       <c r="S23" t="inlineStr"/>
       <c r="T23" t="inlineStr"/>
-      <c r="U23" t="inlineStr"/>
-      <c r="V23" t="inlineStr"/>
-      <c r="W23" t="inlineStr"/>
-      <c r="X23" t="inlineStr"/>
-      <c r="Y23" t="inlineStr"/>
-      <c r="Z23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1896,12 +1534,6 @@
       <c r="R24" t="inlineStr"/>
       <c r="S24" t="inlineStr"/>
       <c r="T24" t="inlineStr"/>
-      <c r="U24" t="inlineStr"/>
-      <c r="V24" t="inlineStr"/>
-      <c r="W24" t="inlineStr"/>
-      <c r="X24" t="inlineStr"/>
-      <c r="Y24" t="inlineStr"/>
-      <c r="Z24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1946,12 +1578,6 @@
       <c r="R25" t="inlineStr"/>
       <c r="S25" t="inlineStr"/>
       <c r="T25" t="inlineStr"/>
-      <c r="U25" t="inlineStr"/>
-      <c r="V25" t="inlineStr"/>
-      <c r="W25" t="inlineStr"/>
-      <c r="X25" t="inlineStr"/>
-      <c r="Y25" t="inlineStr"/>
-      <c r="Z25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1996,12 +1622,6 @@
       <c r="R26" t="inlineStr"/>
       <c r="S26" t="inlineStr"/>
       <c r="T26" t="inlineStr"/>
-      <c r="U26" t="inlineStr"/>
-      <c r="V26" t="inlineStr"/>
-      <c r="W26" t="inlineStr"/>
-      <c r="X26" t="inlineStr"/>
-      <c r="Y26" t="inlineStr"/>
-      <c r="Z26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2046,12 +1666,6 @@
       <c r="R27" t="inlineStr"/>
       <c r="S27" t="inlineStr"/>
       <c r="T27" t="inlineStr"/>
-      <c r="U27" t="inlineStr"/>
-      <c r="V27" t="inlineStr"/>
-      <c r="W27" t="inlineStr"/>
-      <c r="X27" t="inlineStr"/>
-      <c r="Y27" t="inlineStr"/>
-      <c r="Z27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2096,12 +1710,6 @@
       <c r="R28" t="inlineStr"/>
       <c r="S28" t="inlineStr"/>
       <c r="T28" t="inlineStr"/>
-      <c r="U28" t="inlineStr"/>
-      <c r="V28" t="inlineStr"/>
-      <c r="W28" t="inlineStr"/>
-      <c r="X28" t="inlineStr"/>
-      <c r="Y28" t="inlineStr"/>
-      <c r="Z28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2146,12 +1754,6 @@
       <c r="R29" t="inlineStr"/>
       <c r="S29" t="inlineStr"/>
       <c r="T29" t="inlineStr"/>
-      <c r="U29" t="inlineStr"/>
-      <c r="V29" t="inlineStr"/>
-      <c r="W29" t="inlineStr"/>
-      <c r="X29" t="inlineStr"/>
-      <c r="Y29" t="inlineStr"/>
-      <c r="Z29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2196,12 +1798,6 @@
       <c r="R30" t="inlineStr"/>
       <c r="S30" t="inlineStr"/>
       <c r="T30" t="inlineStr"/>
-      <c r="U30" t="inlineStr"/>
-      <c r="V30" t="inlineStr"/>
-      <c r="W30" t="inlineStr"/>
-      <c r="X30" t="inlineStr"/>
-      <c r="Y30" t="inlineStr"/>
-      <c r="Z30" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>